<commit_message>
Read real variable from PLC - in progress
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952B4333-C16C-49DC-BDC5-B11572A49794}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD0B5B-FCD5-4EA3-8015-22501E299486}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="1968" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Id</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>Warning</t>
+  </si>
+  <si>
+    <t>TI_1</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Tank T1 - Level</t>
+  </si>
+  <si>
+    <t>DB1.DBD6</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -426,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,6 +644,39 @@
       </c>
       <c r="L5" s="1"/>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data collection from PLC - in progress
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD0B5B-FCD5-4EA3-8015-22501E299486}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF80DEB-0110-4EAF-BF5B-0BF030D03266}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="1968" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Id</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Warning</t>
   </si>
   <si>
-    <t>TI_1</t>
-  </si>
-  <si>
     <t>REAL</t>
   </si>
   <si>
@@ -124,6 +121,27 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>LI_1</t>
+  </si>
+  <si>
+    <t>Tank T2 - Level</t>
+  </si>
+  <si>
+    <t>Flow measure on pipe to Tank T2</t>
+  </si>
+  <si>
+    <t>DB1.DBD10</t>
+  </si>
+  <si>
+    <t>DB1.DBD14</t>
+  </si>
+  <si>
+    <t>LI_2</t>
+  </si>
+  <si>
+    <t>FI_1</t>
   </si>
 </sst>
 </file>
@@ -444,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,7 +475,7 @@
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
@@ -649,22 +667,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>13</v>
@@ -674,6 +692,72 @@
         <v>0</v>
       </c>
       <c r="K6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data collect and alarm handling complete
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF80DEB-0110-4EAF-BF5B-0BF030D03266}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAE60BA-71C2-45E3-BCC4-E04ABD0FB69C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1968" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Id</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>FI_1</t>
+  </si>
+  <si>
+    <t>Historian</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,6 +520,9 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -552,7 +558,9 @@
       <c r="K2" s="1">
         <v>1</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -588,7 +596,9 @@
       <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -624,7 +634,9 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -660,7 +672,9 @@
       <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -694,6 +708,9 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -727,6 +744,9 @@
       <c r="K7" s="1">
         <v>0</v>
       </c>
+      <c r="L7" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -759,6 +779,9 @@
       </c>
       <c r="K8" s="1">
         <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add all necessary variables form PLC program
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAE60BA-71C2-45E3-BCC4-E04ABD0FB69C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9833A0E-343F-4A3E-9173-1ACCBAEFBCC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3972" yWindow="1644" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="128">
   <si>
     <t>Id</t>
   </si>
@@ -60,101 +60,371 @@
     <t>AlarmLimitMax</t>
   </si>
   <si>
-    <t>LSH_T1</t>
-  </si>
-  <si>
-    <t>DB1.DBX4.0</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
-    <t>Tank T1 - Very High Level</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
     <t>BOOL</t>
   </si>
   <si>
-    <t>LSL_T1</t>
-  </si>
-  <si>
-    <t>DB1.DBX4.1</t>
-  </si>
-  <si>
-    <t>Tank T1 - Very Low Level</t>
-  </si>
-  <si>
-    <t>LSH_T3</t>
-  </si>
-  <si>
-    <t>DB1.DBX4.2</t>
-  </si>
-  <si>
-    <t>Tank T3 - Very High Level</t>
-  </si>
-  <si>
-    <t>LSL_CH1</t>
-  </si>
-  <si>
-    <t>DB1.DBX4.3</t>
-  </si>
-  <si>
-    <t>Tank Ch1 - Very Low Level</t>
-  </si>
-  <si>
-    <t>Warning</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Historian</t>
+  </si>
+  <si>
+    <t>LSHH_T1</t>
+  </si>
+  <si>
+    <t>LSLL_T1</t>
+  </si>
+  <si>
+    <t>LSHH_T2</t>
+  </si>
+  <si>
+    <t>LSLL_T2</t>
+  </si>
+  <si>
+    <t>LSH_CT</t>
+  </si>
+  <si>
+    <t>LSL_CT</t>
+  </si>
+  <si>
+    <t>DB7.DBX0.0</t>
+  </si>
+  <si>
+    <t>DB7.DBX0.1</t>
+  </si>
+  <si>
+    <t>DB7.DBX0.2</t>
+  </si>
+  <si>
+    <t>DB7.DBX0.3</t>
+  </si>
+  <si>
+    <t>DB7.DBX0.4</t>
+  </si>
+  <si>
+    <t>DB7.DBX0.5</t>
+  </si>
+  <si>
+    <t>AI_1_HHI_ALARM</t>
+  </si>
+  <si>
+    <t>DB21.DBX22.0</t>
+  </si>
+  <si>
+    <t>AI_1_HI_WARN</t>
+  </si>
+  <si>
+    <t>DB21.DBX22.1</t>
+  </si>
+  <si>
+    <t>DB21.DBX22.2</t>
+  </si>
+  <si>
+    <t>DB21.DBX22.3</t>
+  </si>
+  <si>
+    <t>AI_1_LO_WARN</t>
+  </si>
+  <si>
+    <t>AI_1_LLO_ALARM</t>
+  </si>
+  <si>
+    <t>Alarm - Very High Level of pH in Tank 2</t>
+  </si>
+  <si>
+    <t>Warn - High Level of pH in Tank 2</t>
+  </si>
+  <si>
+    <t>Warn - Low Level of pH in Tank 2</t>
+  </si>
+  <si>
+    <t>Alarm - Very Low Level of pH in Tank 2</t>
+  </si>
+  <si>
+    <t>FI_1_HHI_ALARM</t>
+  </si>
+  <si>
+    <t>FI_1_HI_WARN</t>
+  </si>
+  <si>
+    <t>FI_1_LO_WARN</t>
+  </si>
+  <si>
+    <t>FI_1_LLO_ALARM</t>
+  </si>
+  <si>
+    <t>Alarm - Very High flow in the pipe leading to the tank 2</t>
+  </si>
+  <si>
+    <t>Warn - High flow in the pipe leading to the tank 2</t>
+  </si>
+  <si>
+    <t>Warn - Low flow in the pipe leading to the tank 2</t>
+  </si>
+  <si>
+    <t>Alarm - Very Low flow in the pipe leading to the tank 2</t>
+  </si>
+  <si>
+    <t>DB19.DBX22.0</t>
+  </si>
+  <si>
+    <t>DB19.DBX22.1</t>
+  </si>
+  <si>
+    <t>DB19.DBX22.2</t>
+  </si>
+  <si>
+    <t>DB19.DBX22.3</t>
+  </si>
+  <si>
+    <t>FI_2_HHI_ALARM</t>
+  </si>
+  <si>
+    <t>FI_2_HI_WARN</t>
+  </si>
+  <si>
+    <t>FI_2_LO_WARN</t>
+  </si>
+  <si>
+    <t>FI_2_LLO_ALARM</t>
+  </si>
+  <si>
+    <t>Alarm - Very High flow at the end of the line</t>
+  </si>
+  <si>
+    <t>Warn - High flow at the end of the line</t>
+  </si>
+  <si>
+    <t>Warn - Low flow at the end of the line</t>
+  </si>
+  <si>
+    <t>Alarm - Very Low flow at the end of the line</t>
+  </si>
+  <si>
+    <t>DB22.DBX22.0</t>
+  </si>
+  <si>
+    <t>DB22.DBX22.1</t>
+  </si>
+  <si>
+    <t>DB22.DBX22.2</t>
+  </si>
+  <si>
+    <t>DB22.DBX22.3</t>
+  </si>
+  <si>
+    <t>DB4.DBX22.0</t>
+  </si>
+  <si>
+    <t>DB4.DBX22.1</t>
+  </si>
+  <si>
+    <t>DB4.DBX22.2</t>
+  </si>
+  <si>
+    <t>DB4.DBX22.3</t>
+  </si>
+  <si>
+    <t>LI_1_HHI_ALARM</t>
+  </si>
+  <si>
+    <t>LI_1_HI_WARN</t>
+  </si>
+  <si>
+    <t>LI_1_LO_WARN</t>
+  </si>
+  <si>
+    <t>LI_1_LLO_ALARM</t>
+  </si>
+  <si>
+    <t>Alarm - Very High level in Tank 1</t>
+  </si>
+  <si>
+    <t>Warn - High level in Tank 1</t>
+  </si>
+  <si>
+    <t>Warn - Low level in Tank 1</t>
+  </si>
+  <si>
+    <t>Alarm - Very Low level in Tank 1</t>
+  </si>
+  <si>
+    <t>LSHH_Tank T1 - Very High Level</t>
+  </si>
+  <si>
+    <t>LSLL_Tank T1 - Very Low Level</t>
+  </si>
+  <si>
+    <t>LSLL_Tank T2 - Very Low Level</t>
+  </si>
+  <si>
+    <t>LSH_Chemicals Tank - High Level</t>
+  </si>
+  <si>
+    <t>LSL_Chemicals Tank - Low Level</t>
+  </si>
+  <si>
+    <t>LSHH_Tank T2 - Very High Level</t>
+  </si>
+  <si>
+    <t>DB20.DBX22.0</t>
+  </si>
+  <si>
+    <t>DB20.DBX22.1</t>
+  </si>
+  <si>
+    <t>DB20.DBX22.2</t>
+  </si>
+  <si>
+    <t>DB20.DBX22.3</t>
+  </si>
+  <si>
+    <t>LI_2_HHI_ALARM</t>
+  </si>
+  <si>
+    <t>LI_2_HI_WARN</t>
+  </si>
+  <si>
+    <t>LI_2_LO_WARN</t>
+  </si>
+  <si>
+    <t>LI_2_LLO_ALARM</t>
+  </si>
+  <si>
+    <t>Alarm - Very High level in Tank 2</t>
+  </si>
+  <si>
+    <t>Warn - High level in Tank 2</t>
+  </si>
+  <si>
+    <t>Warn - Low level in Tank 2</t>
+  </si>
+  <si>
+    <t>Alarm - Very Low level in Tank 2</t>
+  </si>
+  <si>
+    <t>P1_FAULT</t>
+  </si>
+  <si>
+    <t>DB8.DBX6.1</t>
+  </si>
+  <si>
+    <t>Pump P1 - Fault</t>
+  </si>
+  <si>
+    <t>P2_FAULT</t>
+  </si>
+  <si>
+    <t>DB9.DBX6.1</t>
+  </si>
+  <si>
+    <t>Pump P2 - Fault</t>
+  </si>
+  <si>
+    <t>Pump P3 - Fault</t>
+  </si>
+  <si>
+    <t>UV_1_FAULT</t>
+  </si>
+  <si>
+    <t>UV_2_FAULT</t>
+  </si>
+  <si>
+    <t>P3_FAULT</t>
+  </si>
+  <si>
+    <t>DB15.DBX6.1</t>
+  </si>
+  <si>
+    <t>DB10.DBX6.0</t>
+  </si>
+  <si>
+    <t>DB11.DBX6.0</t>
+  </si>
+  <si>
+    <t>UV_1 - Fault</t>
+  </si>
+  <si>
+    <t>UV_2 - Fault</t>
+  </si>
+  <si>
+    <t>AI_1</t>
+  </si>
+  <si>
+    <t>DB29.DBD20.0</t>
   </si>
   <si>
     <t>REAL</t>
   </si>
   <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>Ph in Tank 3</t>
+  </si>
+  <si>
+    <t>FI_1</t>
+  </si>
+  <si>
+    <t>DB5.DBD20.0</t>
+  </si>
+  <si>
+    <t>FI_2</t>
+  </si>
+  <si>
+    <t>LI_1</t>
+  </si>
+  <si>
+    <t>LI_2</t>
+  </si>
+  <si>
+    <t>DB30.DBD20.0</t>
+  </si>
+  <si>
+    <t>DB1.DBD20.0</t>
+  </si>
+  <si>
+    <t>DB28.DBD20.0</t>
+  </si>
+  <si>
+    <t>m3/h</t>
+  </si>
+  <si>
     <t>%</t>
   </si>
   <si>
-    <t>Tank T1 - Level</t>
-  </si>
-  <si>
-    <t>DB1.DBD6</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>LI_1</t>
-  </si>
-  <si>
-    <t>Tank T2 - Level</t>
-  </si>
-  <si>
-    <t>Flow measure on pipe to Tank T2</t>
-  </si>
-  <si>
-    <t>DB1.DBD10</t>
-  </si>
-  <si>
-    <t>DB1.DBD14</t>
-  </si>
-  <si>
-    <t>LI_2</t>
-  </si>
-  <si>
-    <t>FI_1</t>
-  </si>
-  <si>
-    <t>Historian</t>
+    <t>Flow in the pipe leading to the tank 2</t>
+  </si>
+  <si>
+    <t>Flow at the end of the line</t>
+  </si>
+  <si>
+    <t>Tank 1 Level</t>
+  </si>
+  <si>
+    <t>Tank 2 Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,17 +735,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B38" sqref="A38:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
@@ -521,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -529,28 +799,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -559,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -570,25 +840,25 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -597,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -605,28 +875,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -635,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -643,28 +913,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -673,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -681,35 +951,37 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -717,35 +989,37 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -753,38 +1027,1113 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>15</v>
+      <c r="B37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new images. Test Tank progress bar and valve states
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9833A0E-343F-4A3E-9173-1ACCBAEFBCC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22BE66A-77B0-4355-A720-A9A7FC8F2B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3972" yWindow="1644" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="145">
   <si>
     <t>Id</t>
   </si>
@@ -409,6 +409,57 @@
   </si>
   <si>
     <t>Tank 2 Level</t>
+  </si>
+  <si>
+    <t>P1_STATE</t>
+  </si>
+  <si>
+    <t>DB8.DBW10</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Pump P1 - State</t>
+  </si>
+  <si>
+    <t>P2_STATE</t>
+  </si>
+  <si>
+    <t>DB9.DBW10</t>
+  </si>
+  <si>
+    <t>DB15.DBW10</t>
+  </si>
+  <si>
+    <t>P3_STATE</t>
+  </si>
+  <si>
+    <t>Pump P2 - State</t>
+  </si>
+  <si>
+    <t>Pump P3 - State</t>
+  </si>
+  <si>
+    <t>UV_1_STATE</t>
+  </si>
+  <si>
+    <t>DB10.DBW4</t>
+  </si>
+  <si>
+    <t>UV_1 - State</t>
+  </si>
+  <si>
+    <t>UV_2_STATE</t>
+  </si>
+  <si>
+    <t>DB11.DBW4</t>
+  </si>
+  <si>
+    <t>UV_2 - State</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -735,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B38" sqref="A38:B38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1825,28 +1876,26 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J29" s="1">
         <v>0</v>
@@ -1863,10 +1912,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>13</v>
@@ -1875,7 +1924,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>12</v>
@@ -1884,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J30" s="1">
         <v>0</v>
@@ -1901,28 +1950,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="J31" s="1">
         <v>0</v>
@@ -1939,10 +1986,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>13</v>
@@ -1951,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>12</v>
@@ -1960,7 +2007,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J32" s="1">
         <v>0</v>
@@ -1977,31 +2024,35 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="J33" s="1">
         <v>0</v>
       </c>
       <c r="K33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2009,31 +2060,37 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="J34" s="1">
         <v>0</v>
       </c>
       <c r="K34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2041,31 +2098,35 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="J35" s="1">
         <v>0</v>
       </c>
       <c r="K35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2073,31 +2134,37 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="J36" s="1">
         <v>0</v>
       </c>
       <c r="K36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -2105,30 +2172,194 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="1">
-        <v>0</v>
-      </c>
-      <c r="K37" s="1">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1" t="s">
+      <c r="G42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Preparing valve station and do some tests with PLC
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22BE66A-77B0-4355-A720-A9A7FC8F2B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414FCFA-152F-45DF-91E5-4CA7DE3EF721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="159">
   <si>
     <t>Id</t>
   </si>
@@ -444,22 +444,64 @@
     <t>UV_1_STATE</t>
   </si>
   <si>
-    <t>DB10.DBW4</t>
-  </si>
-  <si>
     <t>UV_1 - State</t>
   </si>
   <si>
     <t>UV_2_STATE</t>
   </si>
   <si>
-    <t>DB11.DBW4</t>
-  </si>
-  <si>
     <t>UV_2 - State</t>
   </si>
   <si>
     <t>INT</t>
+  </si>
+  <si>
+    <t>UV_1_MODE</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.1</t>
+  </si>
+  <si>
+    <t>0 - Auto, 1 -  Manual</t>
+  </si>
+  <si>
+    <t>UV_2_MODE</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.1</t>
+  </si>
+  <si>
+    <t>UV_1_OPEN_CLOSE</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.0</t>
+  </si>
+  <si>
+    <t>0 - Close, 1 - Open</t>
+  </si>
+  <si>
+    <t>UV_2_OPEN_CLOSE</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.0</t>
+  </si>
+  <si>
+    <t>UV_1_BLOCKADE</t>
+  </si>
+  <si>
+    <t>DB10.DBW14</t>
+  </si>
+  <si>
+    <t>DB11.DBW14</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.3</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.3</t>
+  </si>
+  <si>
+    <t>UV_2_BLOCKADE</t>
   </si>
 </sst>
 </file>
@@ -786,16 +828,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.21875" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
@@ -1956,7 +1998,7 @@
         <v>133</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
@@ -2030,7 +2072,7 @@
         <v>134</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>11</v>
@@ -2101,23 +2143,23 @@
         <v>138</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J35" s="1">
         <v>0</v>
@@ -2172,26 +2214,26 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J37" s="1">
         <v>0</v>
@@ -2229,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>12</v>
@@ -2261,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>12</v>
@@ -2293,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>12</v>
@@ -2325,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>12</v>
@@ -2357,10 +2399,214 @@
         <v>0</v>
       </c>
       <c r="K42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1">
+        <v>1</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1">
+        <v>1</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <v>1</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Valve station work's fine manual test completed. Cyclic send of data has been added
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414FCFA-152F-45DF-91E5-4CA7DE3EF721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3919881-8AA0-4D8A-8DCF-1672A84B5A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="184">
   <si>
     <t>Id</t>
   </si>
@@ -342,12 +342,6 @@
     <t>DB15.DBX6.1</t>
   </si>
   <si>
-    <t>DB10.DBX6.0</t>
-  </si>
-  <si>
-    <t>DB11.DBX6.0</t>
-  </si>
-  <si>
     <t>UV_1 - Fault</t>
   </si>
   <si>
@@ -456,33 +450,21 @@
     <t>INT</t>
   </si>
   <si>
-    <t>UV_1_MODE</t>
-  </si>
-  <si>
     <t>DB10.DBX12.1</t>
   </si>
   <si>
     <t>0 - Auto, 1 -  Manual</t>
   </si>
   <si>
-    <t>UV_2_MODE</t>
-  </si>
-  <si>
     <t>DB11.DBX12.1</t>
   </si>
   <si>
-    <t>UV_1_OPEN_CLOSE</t>
-  </si>
-  <si>
     <t>DB10.DBX12.0</t>
   </si>
   <si>
     <t>0 - Close, 1 - Open</t>
   </si>
   <si>
-    <t>UV_2_OPEN_CLOSE</t>
-  </si>
-  <si>
     <t>DB11.DBX12.0</t>
   </si>
   <si>
@@ -502,6 +484,99 @@
   </si>
   <si>
     <t>UV_2_BLOCKADE</t>
+  </si>
+  <si>
+    <t>FILL_T1_START</t>
+  </si>
+  <si>
+    <t>DB12.DBX0.0</t>
+  </si>
+  <si>
+    <t>Filling T1 - Start signal from SCADA</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>DB2.DBD0</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.4</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.4</t>
+  </si>
+  <si>
+    <t>UV_1_AM</t>
+  </si>
+  <si>
+    <t>UV_2_AM</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.6</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.6</t>
+  </si>
+  <si>
+    <t>UV_1_OPEN</t>
+  </si>
+  <si>
+    <t>UV_2_OPEN</t>
+  </si>
+  <si>
+    <t>UV_1_CLOSE</t>
+  </si>
+  <si>
+    <t>Open valve UV1 signal from scada</t>
+  </si>
+  <si>
+    <t>Close valve UV1 signal from scada</t>
+  </si>
+  <si>
+    <t>UV_2_CLOSE</t>
+  </si>
+  <si>
+    <t>Close valve UV2 signal from scada</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.5</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.5</t>
+  </si>
+  <si>
+    <t>UV_1_AUTO</t>
+  </si>
+  <si>
+    <t>UV_1_MANUAL</t>
+  </si>
+  <si>
+    <t>DB10.DBX12.2</t>
+  </si>
+  <si>
+    <t>UV_2_AUTO</t>
+  </si>
+  <si>
+    <t>UV_2_MANUAL</t>
+  </si>
+  <si>
+    <t>DB11.DBX12.2</t>
+  </si>
+  <si>
+    <t>UV1 Auto mode signal from scada</t>
+  </si>
+  <si>
+    <t>UV1 Manual mode signal from scada</t>
+  </si>
+  <si>
+    <t>UV2 Auto mode signal from scada</t>
+  </si>
+  <si>
+    <t>UV2 Manual mode signal from scada</t>
   </si>
 </sst>
 </file>
@@ -828,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43:I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,19 +1993,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
@@ -1992,26 +2067,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J31" s="1">
         <v>0</v>
@@ -2066,26 +2141,26 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J33" s="1">
         <v>0</v>
@@ -2105,17 +2180,17 @@
         <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="G34" s="1" t="s">
         <v>12</v>
       </c>
@@ -2123,7 +2198,7 @@
         <v>6</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J34" s="1">
         <v>0</v>
@@ -2140,26 +2215,26 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J35" s="1">
         <v>0</v>
@@ -2179,17 +2254,17 @@
         <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="G36" s="1" t="s">
         <v>12</v>
       </c>
@@ -2197,7 +2272,7 @@
         <v>6</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J36" s="1">
         <v>0</v>
@@ -2214,26 +2289,26 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J37" s="1">
         <v>0</v>
@@ -2250,19 +2325,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>14</v>
@@ -2282,19 +2357,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>14</v>
@@ -2314,19 +2389,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>14</v>
@@ -2346,19 +2421,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>14</v>
@@ -2378,19 +2453,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>14</v>
@@ -2410,10 +2485,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -2422,7 +2497,7 @@
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>14</v>
@@ -2444,10 +2519,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -2456,7 +2531,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
@@ -2478,10 +2553,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -2490,7 +2565,7 @@
         <v>11</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
@@ -2512,10 +2587,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -2524,7 +2599,7 @@
         <v>11</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
@@ -2546,10 +2621,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -2558,7 +2633,7 @@
         <v>11</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>14</v>
@@ -2580,10 +2655,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -2592,7 +2667,7 @@
         <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>14</v>
@@ -2606,6 +2681,277 @@
         <v>1</v>
       </c>
       <c r="L48" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1">
+        <v>1</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <v>1</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
+        <v>1</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+      <c r="K53" s="1">
+        <v>1</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1">
+        <v>1</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1">
+        <v>1</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
+        <v>1</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Pump station and do some manual tests. Still need correct sending real values to PLC
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3919881-8AA0-4D8A-8DCF-1672A84B5A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ECA857-0AB8-4BD6-BBF8-1ABBE87E06E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="217">
   <si>
     <t>Id</t>
   </si>
@@ -312,18 +312,12 @@
     <t>P1_FAULT</t>
   </si>
   <si>
-    <t>DB8.DBX6.1</t>
-  </si>
-  <si>
     <t>Pump P1 - Fault</t>
   </si>
   <si>
     <t>P2_FAULT</t>
   </si>
   <si>
-    <t>DB9.DBX6.1</t>
-  </si>
-  <si>
     <t>Pump P2 - Fault</t>
   </si>
   <si>
@@ -339,9 +333,6 @@
     <t>P3_FAULT</t>
   </si>
   <si>
-    <t>DB15.DBX6.1</t>
-  </si>
-  <si>
     <t>UV_1 - Fault</t>
   </si>
   <si>
@@ -408,24 +399,12 @@
     <t>P1_STATE</t>
   </si>
   <si>
-    <t>DB8.DBW10</t>
-  </si>
-  <si>
-    <t>Int</t>
-  </si>
-  <si>
     <t>Pump P1 - State</t>
   </si>
   <si>
     <t>P2_STATE</t>
   </si>
   <si>
-    <t>DB9.DBW10</t>
-  </si>
-  <si>
-    <t>DB15.DBW10</t>
-  </si>
-  <si>
     <t>P3_STATE</t>
   </si>
   <si>
@@ -577,6 +556,126 @@
   </si>
   <si>
     <t>UV2 Manual mode signal from scada</t>
+  </si>
+  <si>
+    <t>Send</t>
+  </si>
+  <si>
+    <t>P1_AUTO</t>
+  </si>
+  <si>
+    <t>P1_MANUAL</t>
+  </si>
+  <si>
+    <t>P1_START</t>
+  </si>
+  <si>
+    <t>P1_STOP</t>
+  </si>
+  <si>
+    <t>P1_BLOCKADE</t>
+  </si>
+  <si>
+    <t>DB8.DBX18.2</t>
+  </si>
+  <si>
+    <t>DB8.DBX18.3</t>
+  </si>
+  <si>
+    <t>DB8.DBX18.0</t>
+  </si>
+  <si>
+    <t>DB8.DBX18.1</t>
+  </si>
+  <si>
+    <t>DB8.DBX18.4</t>
+  </si>
+  <si>
+    <t>Start signal from Scada</t>
+  </si>
+  <si>
+    <t>Auto mode signal from Scada</t>
+  </si>
+  <si>
+    <t>Manual mode signal from Scada</t>
+  </si>
+  <si>
+    <t>Stop signal from Scada</t>
+  </si>
+  <si>
+    <t>0 - blockade unactive, 1 - blockade active</t>
+  </si>
+  <si>
+    <t>P1_RUN_H</t>
+  </si>
+  <si>
+    <t>P1_RUN_M</t>
+  </si>
+  <si>
+    <t>P1_RUN_S</t>
+  </si>
+  <si>
+    <t>DB8.DBX18.5</t>
+  </si>
+  <si>
+    <t>DB9.DBX18.5</t>
+  </si>
+  <si>
+    <t>DB15.DBX18.5</t>
+  </si>
+  <si>
+    <t>DB8.DBW28</t>
+  </si>
+  <si>
+    <t>DB9.DBW28</t>
+  </si>
+  <si>
+    <t>DB15.DBW28</t>
+  </si>
+  <si>
+    <t>DB8.DBW20</t>
+  </si>
+  <si>
+    <t>DB8.DBW22</t>
+  </si>
+  <si>
+    <t>DB8.DBW24</t>
+  </si>
+  <si>
+    <t>Running time - hours</t>
+  </si>
+  <si>
+    <t>Running time - minutes</t>
+  </si>
+  <si>
+    <t>Running time - seconds</t>
+  </si>
+  <si>
+    <t>P1_SP</t>
+  </si>
+  <si>
+    <t>Setpoint value [%]</t>
+  </si>
+  <si>
+    <t>DB8.DBD30</t>
+  </si>
+  <si>
+    <t>P1_PV</t>
+  </si>
+  <si>
+    <t>Acctual speed [%]</t>
+  </si>
+  <si>
+    <t>DB8.DBD34</t>
+  </si>
+  <si>
+    <t>P1_MODE</t>
+  </si>
+  <si>
+    <t>DB8.DBX26.1</t>
+  </si>
+  <si>
+    <t>0 - auto, 1 - manual (Scada)</t>
   </si>
 </sst>
 </file>
@@ -903,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43:I56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1958,16 +2057,16 @@
         <v>94</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>12</v>
@@ -1976,7 +2075,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J28" s="1">
         <v>0</v>
@@ -1993,26 +2092,26 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>127</v>
+        <v>199</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J29" s="1">
         <v>0</v>
@@ -2029,19 +2128,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>12</v>
@@ -2050,7 +2149,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J30" s="1">
         <v>0</v>
@@ -2067,26 +2166,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="J31" s="1">
         <v>0</v>
@@ -2103,10 +2202,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>104</v>
+        <v>198</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>13</v>
@@ -2115,7 +2214,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>12</v>
@@ -2124,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J32" s="1">
         <v>0</v>
@@ -2141,26 +2240,26 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="E33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J33" s="1">
         <v>0</v>
@@ -2177,10 +2276,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>13</v>
@@ -2189,7 +2288,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>12</v>
@@ -2198,7 +2297,7 @@
         <v>6</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J34" s="1">
         <v>0</v>
@@ -2215,26 +2314,26 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="J35" s="1">
         <v>0</v>
@@ -2251,10 +2350,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>13</v>
@@ -2263,7 +2362,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>12</v>
@@ -2272,7 +2371,7 @@
         <v>6</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J36" s="1">
         <v>0</v>
@@ -2289,26 +2388,26 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="J37" s="1">
         <v>0</v>
@@ -2325,19 +2424,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>14</v>
@@ -2357,19 +2456,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>14</v>
@@ -2389,19 +2488,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>14</v>
@@ -2421,19 +2520,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>14</v>
@@ -2453,19 +2552,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>14</v>
@@ -2485,10 +2584,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -2497,7 +2596,7 @@
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>14</v>
@@ -2519,10 +2618,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -2531,7 +2630,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
@@ -2553,19 +2652,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
@@ -2587,19 +2686,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
@@ -2621,19 +2720,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>14</v>
@@ -2655,19 +2754,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>14</v>
@@ -2689,10 +2788,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
@@ -2701,7 +2800,7 @@
         <v>11</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>14</v>
@@ -2723,10 +2822,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -2735,7 +2834,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>14</v>
@@ -2757,19 +2856,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>14</v>
@@ -2791,19 +2890,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>14</v>
@@ -2825,19 +2924,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F53" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>14</v>
@@ -2859,19 +2958,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
@@ -2893,19 +2992,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
@@ -2927,19 +3026,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
@@ -2952,6 +3051,378 @@
         <v>1</v>
       </c>
       <c r="L56" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1">
+        <v>1</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1">
+        <v>1</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1">
+        <v>1</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1">
+        <v>0</v>
+      </c>
+      <c r="K60" s="1">
+        <v>1</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <v>1</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1">
+        <v>1</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1">
+        <v>1</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1">
+        <v>1</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1">
+        <v>1</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1">
+        <v>1</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>57</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1">
+        <v>1</v>
+      </c>
+      <c r="L67" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add cyclic send real values to PLC. Create template of automation control station
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ECA857-0AB8-4BD6-BBF8-1ABBE87E06E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD2754B-3AFF-405E-B59C-B61B726461CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="262">
   <si>
     <t>Id</t>
   </si>
@@ -676,6 +676,141 @@
   </si>
   <si>
     <t>0 - auto, 1 - manual (Scada)</t>
+  </si>
+  <si>
+    <t>P2_AUTO</t>
+  </si>
+  <si>
+    <t>P2_MANUAL</t>
+  </si>
+  <si>
+    <t>P2_START</t>
+  </si>
+  <si>
+    <t>P2_STOP</t>
+  </si>
+  <si>
+    <t>P2_BLOCKADE</t>
+  </si>
+  <si>
+    <t>P2_RUN_H</t>
+  </si>
+  <si>
+    <t>P2_RUN_M</t>
+  </si>
+  <si>
+    <t>P2_RUN_S</t>
+  </si>
+  <si>
+    <t>P2_SP</t>
+  </si>
+  <si>
+    <t>P2_PV</t>
+  </si>
+  <si>
+    <t>P2_MODE</t>
+  </si>
+  <si>
+    <t>DB9.DBX18.2</t>
+  </si>
+  <si>
+    <t>DB9.DBX18.3</t>
+  </si>
+  <si>
+    <t>DB9.DBX18.0</t>
+  </si>
+  <si>
+    <t>DB9.DBX18.1</t>
+  </si>
+  <si>
+    <t>DB9.DBX18.4</t>
+  </si>
+  <si>
+    <t>DB9.DBW20</t>
+  </si>
+  <si>
+    <t>DB9.DBW22</t>
+  </si>
+  <si>
+    <t>DB9.DBW24</t>
+  </si>
+  <si>
+    <t>DB9.DBD30</t>
+  </si>
+  <si>
+    <t>DB9.DBD34</t>
+  </si>
+  <si>
+    <t>DB9.DBX26.1</t>
+  </si>
+  <si>
+    <t>P3_AUTO</t>
+  </si>
+  <si>
+    <t>P3_MANUAL</t>
+  </si>
+  <si>
+    <t>P3_START</t>
+  </si>
+  <si>
+    <t>P3_BLOCKADE</t>
+  </si>
+  <si>
+    <t>P3_RUN_H</t>
+  </si>
+  <si>
+    <t>P3_RUN_M</t>
+  </si>
+  <si>
+    <t>P3_RUN_S</t>
+  </si>
+  <si>
+    <t>P3_SP</t>
+  </si>
+  <si>
+    <t>P3_PV</t>
+  </si>
+  <si>
+    <t>P3_MODE</t>
+  </si>
+  <si>
+    <t>DB15.DBX18.2</t>
+  </si>
+  <si>
+    <t>DB15.DBX18.3</t>
+  </si>
+  <si>
+    <t>DB15.DBX18.0</t>
+  </si>
+  <si>
+    <t>DB15.DBX18.1</t>
+  </si>
+  <si>
+    <t>DB15.DBX18.4</t>
+  </si>
+  <si>
+    <t>DB15.DBW20</t>
+  </si>
+  <si>
+    <t>DB15.DBW22</t>
+  </si>
+  <si>
+    <t>DB15.DBW24</t>
+  </si>
+  <si>
+    <t>DB15.DBD30</t>
+  </si>
+  <si>
+    <t>DB15.DBD34</t>
+  </si>
+  <si>
+    <t>DB15.DBX26.1</t>
+  </si>
+  <si>
+    <t>TestInt</t>
+  </si>
+  <si>
+    <t>DB2.DBW4</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3394,7 +3529,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>214</v>
@@ -3423,6 +3558,784 @@
         <v>1</v>
       </c>
       <c r="L67" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1">
+        <v>1</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1">
+        <v>0</v>
+      </c>
+      <c r="K69" s="1">
+        <v>1</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1">
+        <v>1</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1">
+        <v>1</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1">
+        <v>0</v>
+      </c>
+      <c r="K72" s="1">
+        <v>1</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+      <c r="K73" s="1">
+        <v>1</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1">
+        <v>0</v>
+      </c>
+      <c r="K74" s="1">
+        <v>1</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1">
+        <v>0</v>
+      </c>
+      <c r="K75" s="1">
+        <v>1</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1">
+        <v>0</v>
+      </c>
+      <c r="K76" s="1">
+        <v>1</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1">
+        <v>1</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1">
+        <v>1</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1">
+        <v>1</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+      <c r="K80" s="1">
+        <v>1</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1">
+        <v>0</v>
+      </c>
+      <c r="K81" s="1">
+        <v>1</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1">
+        <v>1</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1">
+        <v>0</v>
+      </c>
+      <c r="K83" s="1">
+        <v>1</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1">
+        <v>0</v>
+      </c>
+      <c r="K84" s="1">
+        <v>1</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1">
+        <v>0</v>
+      </c>
+      <c r="K85" s="1">
+        <v>1</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1">
+        <v>0</v>
+      </c>
+      <c r="K86" s="1">
+        <v>1</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1">
+        <v>0</v>
+      </c>
+      <c r="K87" s="1">
+        <v>1</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1">
+        <v>0</v>
+      </c>
+      <c r="K88" s="1">
+        <v>1</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1">
+        <v>0</v>
+      </c>
+      <c r="K89" s="1">
+        <v>1</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+      <c r="K90" s="1">
+        <v>1</v>
+      </c>
+      <c r="L90" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatic control stations complete. Manual tests are required
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD2754B-3AFF-405E-B59C-B61B726461CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C86C0BE-FD72-4AAA-91FA-779B8BC05186}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="304">
   <si>
     <t>Id</t>
   </si>
@@ -811,6 +811,132 @@
   </si>
   <si>
     <t>DB2.DBW4</t>
+  </si>
+  <si>
+    <t>Start filling signal from SCADA</t>
+  </si>
+  <si>
+    <t>FILL_T1_STOP</t>
+  </si>
+  <si>
+    <t>Stop filling signal from SCADA</t>
+  </si>
+  <si>
+    <t>DB12.DBX0.2</t>
+  </si>
+  <si>
+    <t>FILL_T1_STATE</t>
+  </si>
+  <si>
+    <t>DB12.DBW2</t>
+  </si>
+  <si>
+    <t>0 - Stop, 1 - Filling T1, 2 - No conditions to run</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_T2_START</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_T2_STOP</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_T2_STATE</t>
+  </si>
+  <si>
+    <t>DB18.DBX0.0</t>
+  </si>
+  <si>
+    <t>DB18.DBX0.2</t>
+  </si>
+  <si>
+    <t>Stop transfer to T2 signal from SCADA</t>
+  </si>
+  <si>
+    <t>Start transfer to T2 signal from SCADA</t>
+  </si>
+  <si>
+    <t>0 - Stop, 1 - Transfer to T2, 2 - Adding chemicals, 3 - No conditions to run</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_T2_LI_2_SP</t>
+  </si>
+  <si>
+    <t>DB18.DBW10</t>
+  </si>
+  <si>
+    <t>DB18.DBD2</t>
+  </si>
+  <si>
+    <t>Setpoint for Tank T2 filling level [%]</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_T2_P1_SP</t>
+  </si>
+  <si>
+    <t>DB18.DBD12</t>
+  </si>
+  <si>
+    <t>Pump P1 Speed Setpoint [%]</t>
+  </si>
+  <si>
+    <t>DOSE_CHEMICALS_START</t>
+  </si>
+  <si>
+    <t>DOSE_CHEMICALS_STOP</t>
+  </si>
+  <si>
+    <t>DOSE_CHEMICALS_STATE</t>
+  </si>
+  <si>
+    <t>DB24.DBX0.0</t>
+  </si>
+  <si>
+    <t>DB24.DBX0.2</t>
+  </si>
+  <si>
+    <t>0 - Stop, 1 - Adding Chemicals, 2 - No conditions to run</t>
+  </si>
+  <si>
+    <t>DB24.DBW2</t>
+  </si>
+  <si>
+    <t>Pump P2 Speed Setpoint [%]</t>
+  </si>
+  <si>
+    <t>EMPTYING_T2_P2_SP</t>
+  </si>
+  <si>
+    <t>DB27.DBD4</t>
+  </si>
+  <si>
+    <t>DB27.DBW2</t>
+  </si>
+  <si>
+    <t>DB27.DBX0.2</t>
+  </si>
+  <si>
+    <t>DB27.DBX0.0</t>
+  </si>
+  <si>
+    <t>Start dosing chemicals signal from SCADA</t>
+  </si>
+  <si>
+    <t>Stop dosing chemicals to T2 signal from SCADA</t>
+  </si>
+  <si>
+    <t>Start emptying T2 signal from SCADA</t>
+  </si>
+  <si>
+    <t>Stop emptying T2 signal from SCADA</t>
+  </si>
+  <si>
+    <t>EMPTYING_T2_STATE</t>
+  </si>
+  <si>
+    <t>EMPTYING_T2_STOP</t>
+  </si>
+  <si>
+    <t>EMPTYING_T2_START</t>
   </si>
 </sst>
 </file>
@@ -1137,20 +1263,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:A90"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
     <col min="2" max="2" width="23.109375" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="6" max="6" width="43" customWidth="1"/>
     <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
@@ -4339,6 +4465,513 @@
         <v>14</v>
       </c>
     </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1">
+        <v>0</v>
+      </c>
+      <c r="K91" s="1">
+        <v>1</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1">
+        <v>0</v>
+      </c>
+      <c r="K92" s="1">
+        <v>1</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1">
+        <v>0</v>
+      </c>
+      <c r="K93" s="1">
+        <v>1</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1">
+        <v>0</v>
+      </c>
+      <c r="K94" s="1">
+        <v>1</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1">
+        <v>1</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+      <c r="K96" s="1">
+        <v>1</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1">
+        <v>0</v>
+      </c>
+      <c r="K97" s="1">
+        <v>1</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1">
+        <v>0</v>
+      </c>
+      <c r="K98" s="1">
+        <v>1</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1">
+        <v>0</v>
+      </c>
+      <c r="K99" s="1">
+        <v>1</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1">
+        <v>0</v>
+      </c>
+      <c r="K100" s="1">
+        <v>1</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1">
+        <v>0</v>
+      </c>
+      <c r="K101" s="1">
+        <v>1</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1">
+        <v>1</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1">
+        <v>0</v>
+      </c>
+      <c r="K103" s="1">
+        <v>1</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1">
+        <v>0</v>
+      </c>
+      <c r="K104" s="1">
+        <v>1</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1">
+        <v>0</v>
+      </c>
+      <c r="K105" s="1">
+        <v>1</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add process graphic visualisation
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C86C0BE-FD72-4AAA-91FA-779B8BC05186}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D1217E-E1CB-433C-8751-FBE548AD1661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:L105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:A105"/>
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix decimapl places in values. Change imgs source paths. Add SimpleScada logo. Test PLC programm with visualisation
</commit_message>
<xml_diff>
--- a/Excel/Variables.xlsx
+++ b/Excel/Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programowanie\WPF\ProjektScadaMes\SimpleScada\SimpleScada\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D1217E-E1CB-433C-8751-FBE548AD1661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD666AFD-6D94-4926-A447-89B715712F10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="2808" windowWidth="15336" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="301">
   <si>
     <t>Id</t>
   </si>
@@ -372,12 +372,6 @@
     <t>DB30.DBD20.0</t>
   </si>
   <si>
-    <t>DB1.DBD20.0</t>
-  </si>
-  <si>
-    <t>DB28.DBD20.0</t>
-  </si>
-  <si>
     <t>m3/h</t>
   </si>
   <si>
@@ -858,18 +852,9 @@
     <t>0 - Stop, 1 - Transfer to T2, 2 - Adding chemicals, 3 - No conditions to run</t>
   </si>
   <si>
-    <t>TRANSFER_TO_T2_LI_2_SP</t>
-  </si>
-  <si>
     <t>DB18.DBW10</t>
   </si>
   <si>
-    <t>DB18.DBD2</t>
-  </si>
-  <si>
-    <t>Setpoint for Tank T2 filling level [%]</t>
-  </si>
-  <si>
     <t>TRANSFER_TO_T2_P1_SP</t>
   </si>
   <si>
@@ -937,6 +922,12 @@
   </si>
   <si>
     <t>EMPTYING_T2_START</t>
+  </si>
+  <si>
+    <t>DB23.DBD8.0</t>
+  </si>
+  <si>
+    <t>DB6.DBD8.0</t>
   </si>
 </sst>
 </file>
@@ -1263,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2318,7 +2309,7 @@
         <v>94</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>13</v>
@@ -2353,19 +2344,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
@@ -2392,7 +2383,7 @@
         <v>96</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>13</v>
@@ -2427,26 +2418,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J31" s="1">
         <v>0</v>
@@ -2466,7 +2457,7 @@
         <v>101</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>13</v>
@@ -2501,26 +2492,26 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J33" s="1">
         <v>0</v>
@@ -2540,7 +2531,7 @@
         <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>13</v>
@@ -2575,26 +2566,26 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J35" s="1">
         <v>0</v>
@@ -2614,7 +2605,7 @@
         <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>13</v>
@@ -2649,26 +2640,26 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J37" s="1">
         <v>0</v>
@@ -2726,10 +2717,10 @@
         <v>106</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>14</v>
@@ -2758,10 +2749,10 @@
         <v>106</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>14</v>
@@ -2784,16 +2775,16 @@
         <v>112</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>115</v>
+        <v>299</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>14</v>
@@ -2816,16 +2807,16 @@
         <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>116</v>
+        <v>300</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>14</v>
@@ -2845,10 +2836,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -2857,7 +2848,7 @@
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>14</v>
@@ -2879,10 +2870,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -2891,7 +2882,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
@@ -2913,19 +2904,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
@@ -2947,19 +2938,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
@@ -2981,19 +2972,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>14</v>
@@ -3015,19 +3006,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>14</v>
@@ -3049,10 +3040,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
@@ -3061,7 +3052,7 @@
         <v>11</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>14</v>
@@ -3083,10 +3074,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -3095,7 +3086,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>14</v>
@@ -3117,19 +3108,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>14</v>
@@ -3151,19 +3142,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>14</v>
@@ -3185,19 +3176,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>14</v>
@@ -3219,19 +3210,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
@@ -3253,19 +3244,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
@@ -3287,10 +3278,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>106</v>
@@ -3299,7 +3290,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
@@ -3320,19 +3311,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
@@ -3354,19 +3345,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
@@ -3388,19 +3379,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>14</v>
@@ -3422,19 +3413,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>14</v>
@@ -3456,10 +3447,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>13</v>
@@ -3468,7 +3459,7 @@
         <v>11</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>14</v>
@@ -3490,19 +3481,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>14</v>
@@ -3524,19 +3515,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>14</v>
@@ -3558,19 +3549,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>14</v>
@@ -3592,19 +3583,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
@@ -3625,10 +3616,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>106</v>
@@ -3637,7 +3628,7 @@
         <v>11</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
@@ -3658,19 +3649,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
@@ -3692,19 +3683,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>14</v>
@@ -3726,19 +3717,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>14</v>
@@ -3760,19 +3751,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>14</v>
@@ -3794,19 +3785,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>14</v>
@@ -3828,10 +3819,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>13</v>
@@ -3840,7 +3831,7 @@
         <v>11</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>14</v>
@@ -3862,19 +3853,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>14</v>
@@ -3896,19 +3887,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>14</v>
@@ -3930,19 +3921,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>14</v>
@@ -3964,19 +3955,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>14</v>
@@ -3997,10 +3988,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>106</v>
@@ -4009,7 +4000,7 @@
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>14</v>
@@ -4030,10 +4021,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -4042,7 +4033,7 @@
         <v>11</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>14</v>
@@ -4064,19 +4055,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>14</v>
@@ -4098,19 +4089,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>14</v>
@@ -4132,19 +4123,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>14</v>
@@ -4166,19 +4157,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>14</v>
@@ -4200,10 +4191,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>13</v>
@@ -4212,7 +4203,7 @@
         <v>11</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>14</v>
@@ -4234,19 +4225,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>14</v>
@@ -4268,19 +4259,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>14</v>
@@ -4302,19 +4293,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>14</v>
@@ -4336,19 +4327,19 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>14</v>
@@ -4369,10 +4360,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>106</v>
@@ -4381,7 +4372,7 @@
         <v>11</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>14</v>
@@ -4402,10 +4393,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>13</v>
@@ -4414,7 +4405,7 @@
         <v>11</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>14</v>
@@ -4436,19 +4427,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>14</v>
@@ -4470,19 +4461,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>14</v>
@@ -4504,19 +4495,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="D92" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>14</v>
@@ -4538,19 +4529,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>14</v>
@@ -4572,19 +4563,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>14</v>
@@ -4606,19 +4597,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>14</v>
@@ -4640,19 +4631,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>14</v>
@@ -4671,22 +4662,22 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>14</v>
@@ -4704,26 +4695,27 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>282</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1">
         <v>0</v>
@@ -4737,22 +4729,22 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>14</v>
@@ -4771,22 +4763,22 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="D100" s="1" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>14</v>
@@ -4805,22 +4797,22 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>14</v>
@@ -4839,22 +4831,22 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>14</v>
@@ -4873,22 +4865,22 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>14</v>
@@ -4907,27 +4899,26 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1">
         <v>0</v>
@@ -4936,39 +4927,6 @@
         <v>1</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
-        <v>104</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1">
-        <v>0</v>
-      </c>
-      <c r="K105" s="1">
-        <v>1</v>
-      </c>
-      <c r="L105" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>